<commit_message>
Cập nhật thay đổi giá trị ngày năm năm liên tục
</commit_message>
<xml_diff>
--- a/XML130/File-ho-tro/postgres-table.xlsx
+++ b/XML130/File-ho-tro/postgres-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLOUDCODE\github.com\dh-hos\Mo-ta-he-thong\XML130\File-ho-tro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1A995E-06F6-4D10-9249-47FAF906D2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CA28F4-C02F-40FE-B181-04C8EBE142D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{BD06A603-30CD-466B-9364-E8E1CF938873}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15450" firstSheet="1" activeTab="7" xr2:uid="{BD06A603-30CD-466B-9364-E8E1CF938873}"/>
   </bookViews>
   <sheets>
     <sheet name="current.psgiamdinhykhoa" sheetId="1" r:id="rId1"/>
@@ -1133,12 +1133,6 @@
 Cột bổ sung mới. can_nang_con = sumtext(ttcon.cannang)</t>
   </si>
   <si>
-    <t>Ghi thời điểm người bệnh tham gia BHYT đủ 05 năm liên tục, gồm 08 ký tự theo định dạng yyyymmdd.
-Cột bổ sung mới.
--	Khám ngoại trú: nam_nam_lien_tuc = to_char(psdangky.ngay55lientuc, 'yyyyMMyy').
--	Nội trú/BA ngoại trú cuối đợt: nam_nam_lien_tuc = to_char(bnnoitru.ngay55lientuc, 'yyyyMMyy') đối với thẻ 1. nam_nam_lien_tuc = to_char(ttcon.ngay55lientuc, 'yyyyMMyy') đối với thẻ 2.</t>
-  </si>
-  <si>
     <t>Ghi ngày cơ sở KBCB hẹn người bệnh tái khám tiếp theo (nếu có), gồm 08 ký tự theo định dạng yyyymmdd. 
 Trường hợp người bệnh được cơ sở KBCB hẹn nhiều ngày tái khám khác nhau (người bệnh được chỉ định khám nhiều hơn 01 chuyên khoa trong một đợt KBCB) thì giữa các ngày tái khám cách nhau bằng dấu chấm phẩy “;”.
 Cột bổ sung mới. Chỉ áp dụng đối với khám ngoại trú: ngay_tai_kham = to_char(psdangky.ngaytaikham, 'yyyyMMyy')</t>
@@ -2951,6 +2945,12 @@
   </si>
   <si>
     <t>psgiamdinhykhoa.mabn</t>
+  </si>
+  <si>
+    <t>Ghi thời điểm người bệnh tham gia BHYT đủ 05 năm liên tục, gồm 08 ký tự theo định dạng yyyymmdd.
+Cột bổ sung mới.
+-	Khám ngoại trú: nam_nam_lien_tuc = to_char(psdangky.ngay5nam, 'yyyyMMyy').
+-	Nội trú/BA ngoại trú cuối đợt: nam_nam_lien_tuc = to_char(bnnoitru.ngay5nam, 'yyyyMMyy') đối với thẻ 1. nam_nam_lien_tuc = to_char(ttcon.ngay55lientuc, 'yyyyMMyy') đối với thẻ 2.</t>
   </si>
 </sst>
 </file>
@@ -3956,7 +3956,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>27</v>
@@ -3965,7 +3965,7 @@
         <v>213</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>88</v>
@@ -3979,7 +3979,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>27</v>
@@ -3988,7 +3988,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -4002,7 +4002,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>27</v>
@@ -4011,7 +4011,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -4034,7 +4034,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -4057,7 +4057,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -4071,7 +4071,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>14</v>
@@ -4080,7 +4080,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -4094,7 +4094,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>44</v>
@@ -4103,7 +4103,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -4117,7 +4117,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>78</v>
@@ -4126,7 +4126,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -4140,7 +4140,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>158</v>
@@ -4149,7 +4149,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -4166,13 +4166,13 @@
         <v>172</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -4186,16 +4186,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -4212,13 +4212,13 @@
         <v>189</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -4241,7 +4241,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -4255,7 +4255,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>27</v>
@@ -4264,7 +4264,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -4278,7 +4278,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>17</v>
@@ -4287,7 +4287,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -4301,7 +4301,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>210</v>
@@ -4310,7 +4310,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>88</v>
@@ -4324,7 +4324,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>215</v>
@@ -4333,7 +4333,7 @@
         <v>88</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -4347,7 +4347,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>215</v>
@@ -4356,7 +4356,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -4370,7 +4370,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>76</v>
@@ -4379,7 +4379,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -4393,7 +4393,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>17</v>
@@ -4402,7 +4402,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -4416,7 +4416,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>17</v>
@@ -4425,7 +4425,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -4439,7 +4439,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>158</v>
@@ -4448,7 +4448,7 @@
         <v>88</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>88</v>
@@ -4462,7 +4462,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>210</v>
@@ -4471,7 +4471,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>88</v>
@@ -4485,7 +4485,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>210</v>
@@ -4494,7 +4494,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>88</v>
@@ -4515,7 +4515,7 @@
         <v>8</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>8</v>
@@ -4625,7 +4625,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>88</v>
@@ -4639,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>17</v>
@@ -4648,7 +4648,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -4662,7 +4662,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>17</v>
@@ -4671,7 +4671,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -4685,7 +4685,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>17</v>
@@ -4694,7 +4694,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -4708,7 +4708,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>41</v>
@@ -4717,7 +4717,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -4740,7 +4740,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -4763,7 +4763,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -4786,7 +4786,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -4809,7 +4809,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -4823,7 +4823,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>44</v>
@@ -4832,7 +4832,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -4846,7 +4846,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>44</v>
@@ -4855,7 +4855,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -4869,7 +4869,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>44</v>
@@ -4878,7 +4878,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -4892,7 +4892,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>210</v>
@@ -4901,7 +4901,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -4915,7 +4915,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>210</v>
@@ -4924,7 +4924,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -4938,7 +4938,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>158</v>
@@ -4947,7 +4947,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -4987,13 +4987,13 @@
         <v>189</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -5010,13 +5010,13 @@
         <v>214</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -5030,7 +5030,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>210</v>
@@ -5039,7 +5039,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -5053,7 +5053,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>76</v>
@@ -5062,7 +5062,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -5085,7 +5085,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -5106,7 +5106,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>8</v>
@@ -5196,7 +5196,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>8</v>
@@ -5210,16 +5210,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>88</v>
@@ -5233,7 +5233,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>76</v>
@@ -5242,7 +5242,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -5256,7 +5256,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>17</v>
@@ -5265,7 +5265,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -5279,7 +5279,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>210</v>
@@ -5288,7 +5288,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -5302,7 +5302,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>158</v>
@@ -5311,7 +5311,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -5325,7 +5325,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>155</v>
@@ -5334,7 +5334,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -5348,7 +5348,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>210</v>
@@ -5357,7 +5357,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -5371,7 +5371,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>41</v>
@@ -5380,7 +5380,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -5394,7 +5394,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>41</v>
@@ -5403,7 +5403,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -5426,7 +5426,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -5449,7 +5449,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -5472,7 +5472,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -5495,7 +5495,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -5509,7 +5509,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>17</v>
@@ -5518,7 +5518,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -5532,7 +5532,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>76</v>
@@ -5541,7 +5541,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -5555,7 +5555,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>17</v>
@@ -5564,7 +5564,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>88</v>
@@ -5578,7 +5578,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>14</v>
@@ -5587,7 +5587,7 @@
         <v>8</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -5601,7 +5601,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>158</v>
@@ -5610,7 +5610,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -5624,7 +5624,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>158</v>
@@ -5633,7 +5633,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -5647,7 +5647,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>158</v>
@@ -5656,7 +5656,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -5673,13 +5673,13 @@
         <v>208</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -5693,7 +5693,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>78</v>
@@ -5702,7 +5702,7 @@
         <v>88</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>88</v>
@@ -5716,7 +5716,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>41</v>
@@ -5725,7 +5725,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>88</v>
@@ -5739,7 +5739,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>44</v>
@@ -5748,7 +5748,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>88</v>
@@ -5762,7 +5762,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>14</v>
@@ -5771,7 +5771,7 @@
         <v>88</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>88</v>
@@ -5785,7 +5785,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>14</v>
@@ -5794,7 +5794,7 @@
         <v>88</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>88</v>
@@ -5817,7 +5817,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>88</v>
@@ -5831,7 +5831,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>17</v>
@@ -5840,7 +5840,7 @@
         <v>88</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>88</v>
@@ -5854,7 +5854,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>17</v>
@@ -5863,7 +5863,7 @@
         <v>88</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>88</v>
@@ -5877,7 +5877,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>210</v>
@@ -5886,7 +5886,7 @@
         <v>88</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>88</v>
@@ -5900,7 +5900,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>27</v>
@@ -5909,7 +5909,7 @@
         <v>88</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>88</v>
@@ -5923,7 +5923,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>27</v>
@@ -5932,7 +5932,7 @@
         <v>88</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>88</v>
@@ -5949,13 +5949,13 @@
         <v>214</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>88</v>
@@ -5976,7 +5976,7 @@
         <v>8</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>8</v>
@@ -5997,7 +5997,7 @@
         <v>8</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>8</v>
@@ -6078,7 +6078,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>27</v>
@@ -6087,7 +6087,7 @@
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>88</v>
@@ -6101,7 +6101,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>27</v>
@@ -6110,7 +6110,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -6124,7 +6124,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>30</v>
@@ -6133,7 +6133,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -6147,7 +6147,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>41</v>
@@ -6156,7 +6156,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -6179,7 +6179,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -6193,7 +6193,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>210</v>
@@ -6202,7 +6202,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -6216,7 +6216,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>210</v>
@@ -6225,7 +6225,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -6242,13 +6242,13 @@
         <v>214</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -6262,7 +6262,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>17</v>
@@ -6271,7 +6271,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -6285,7 +6285,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>27</v>
@@ -6294,7 +6294,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -6308,7 +6308,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>210</v>
@@ -6317,7 +6317,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -6338,7 +6338,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>8</v>
@@ -6359,7 +6359,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>8</v>
@@ -6439,7 +6439,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>27</v>
@@ -6448,7 +6448,7 @@
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>88</v>
@@ -6462,7 +6462,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>27</v>
@@ -6471,7 +6471,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -6485,7 +6485,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>27</v>
@@ -6494,13 +6494,13 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="120.75" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>41</v>
@@ -6517,7 +6517,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -6531,22 +6531,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="310.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="276" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -6563,13 +6563,13 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="224.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="189.75" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -6600,7 +6600,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>44</v>
@@ -6609,13 +6609,13 @@
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>14</v>
@@ -6632,7 +6632,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -6646,7 +6646,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>44</v>
@@ -6655,7 +6655,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -6669,7 +6669,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>158</v>
@@ -6678,13 +6678,13 @@
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="155.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>30</v>
@@ -6701,7 +6701,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -6715,7 +6715,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>210</v>
@@ -6724,7 +6724,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -6738,7 +6738,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>210</v>
@@ -6747,7 +6747,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -6761,7 +6761,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>17</v>
@@ -6770,7 +6770,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -6784,7 +6784,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>17</v>
@@ -6793,7 +6793,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>88</v>
@@ -6810,13 +6810,13 @@
         <v>214</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -6830,7 +6830,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>27</v>
@@ -6839,7 +6839,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -6853,7 +6853,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>210</v>
@@ -6862,7 +6862,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -6876,7 +6876,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>76</v>
@@ -6885,7 +6885,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -6899,7 +6899,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>160</v>
@@ -6908,7 +6908,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -6929,7 +6929,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>8</v>
@@ -6950,7 +6950,7 @@
         <v>8</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>8</v>
@@ -7018,7 +7018,7 @@
         <v>88</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G2" s="17"/>
     </row>
@@ -7039,7 +7039,7 @@
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>88</v>
@@ -7062,7 +7062,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -7085,7 +7085,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -7108,7 +7108,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -7131,7 +7131,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -7145,7 +7145,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>210</v>
@@ -7154,7 +7154,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -7168,7 +7168,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>41</v>
@@ -7177,7 +7177,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -7200,7 +7200,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -7223,7 +7223,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -7246,7 +7246,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -7269,7 +7269,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -7283,16 +7283,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -7315,7 +7315,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -7329,7 +7329,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>72</v>
@@ -7338,7 +7338,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -7361,7 +7361,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -7384,7 +7384,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>88</v>
@@ -7407,7 +7407,7 @@
         <v>88</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -7430,7 +7430,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -7453,7 +7453,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -7476,7 +7476,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -7499,7 +7499,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -7522,7 +7522,7 @@
         <v>88</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>88</v>
@@ -7545,7 +7545,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>88</v>
@@ -7568,7 +7568,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>88</v>
@@ -7591,7 +7591,7 @@
         <v>88</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>88</v>
@@ -7614,7 +7614,7 @@
         <v>88</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>88</v>
@@ -7637,7 +7637,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>88</v>
@@ -7660,7 +7660,7 @@
         <v>88</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>88</v>
@@ -7683,7 +7683,7 @@
         <v>88</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>88</v>
@@ -7706,7 +7706,7 @@
         <v>88</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>88</v>
@@ -7729,7 +7729,7 @@
         <v>88</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>88</v>
@@ -7752,7 +7752,7 @@
         <v>88</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>88</v>
@@ -7775,7 +7775,7 @@
         <v>88</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>88</v>
@@ -7798,7 +7798,7 @@
         <v>88</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>88</v>
@@ -7819,7 +7819,7 @@
         <v>8</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>8</v>
@@ -7840,7 +7840,7 @@
         <v>8</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>8</v>
@@ -7861,7 +7861,7 @@
         <v>8</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>8</v>
@@ -8530,8 +8530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD753213-A7AB-4D04-91E1-0D02042F8204}">
   <dimension ref="A2:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B57" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8613,7 +8613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="138" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="155.25" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>3</v>
       </c>
@@ -8636,7 +8636,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>4</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="138" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>5</v>
       </c>
@@ -8728,7 +8728,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>8</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="138" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>9</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>11</v>
       </c>
@@ -8889,7 +8889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="224.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="276" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>15</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="155.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="189.75" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>16</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="155.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="172.5" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>17</v>
       </c>
@@ -8958,7 +8958,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="138" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="189.75" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>18</v>
       </c>
@@ -8981,7 +8981,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="172.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>19</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="241.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="258.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>20</v>
       </c>
@@ -9050,7 +9050,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>22</v>
       </c>
@@ -9096,7 +9096,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="172.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="189.75" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>24</v>
       </c>
@@ -9119,7 +9119,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="120.75" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>25</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="276" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="310.5" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>30</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>32</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>34</v>
       </c>
@@ -9349,7 +9349,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="327.75" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>35</v>
       </c>
@@ -9372,7 +9372,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="120.75" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>36</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>37</v>
       </c>
@@ -9510,7 +9510,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="138" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>42</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>43</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>47</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>48</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>50</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="138" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="155.25" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>54</v>
       </c>
@@ -9809,7 +9809,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="138" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>55</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>88</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>273</v>
+        <v>695</v>
       </c>
       <c r="G62" s="17" t="s">
         <v>88</v>
@@ -9964,7 +9964,7 @@
         <v>88</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G63" s="17" t="s">
         <v>88</v>
@@ -9987,13 +9987,13 @@
         <v>213</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G64" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="69" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>63</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>88</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G65" s="17" t="s">
         <v>88</v>
@@ -10033,7 +10033,7 @@
         <v>88</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G66" s="17" t="s">
         <v>88</v>
@@ -10139,7 +10139,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>17</v>
@@ -10148,7 +10148,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>8</v>
@@ -10162,7 +10162,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>17</v>
@@ -10171,7 +10171,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>88</v>
@@ -10185,7 +10185,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>215</v>
@@ -10194,7 +10194,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>88</v>
@@ -10208,7 +10208,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>158</v>
@@ -10217,7 +10217,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>88</v>
@@ -10231,7 +10231,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>41</v>
@@ -10240,7 +10240,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>88</v>
@@ -10254,7 +10254,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>82</v>
@@ -10263,7 +10263,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>88</v>
@@ -10277,7 +10277,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>41</v>
@@ -10286,7 +10286,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>88</v>
@@ -10300,7 +10300,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>87</v>
@@ -10309,7 +10309,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G10" s="22" t="s">
         <v>88</v>
@@ -10323,7 +10323,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>41</v>
@@ -10332,7 +10332,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G11" s="22" t="s">
         <v>88</v>
@@ -10346,7 +10346,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>41</v>
@@ -10355,7 +10355,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G12" s="22" t="s">
         <v>88</v>
@@ -10369,7 +10369,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>41</v>
@@ -10378,7 +10378,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>88</v>
@@ -10392,7 +10392,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>17</v>
@@ -10401,7 +10401,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>88</v>
@@ -10415,7 +10415,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>82</v>
@@ -10424,7 +10424,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>88</v>
@@ -10438,7 +10438,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>14</v>
@@ -10447,7 +10447,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>88</v>
@@ -10461,7 +10461,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>30</v>
@@ -10470,7 +10470,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>88</v>
@@ -10484,16 +10484,16 @@
         <v>18</v>
       </c>
       <c r="C18" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>294</v>
-      </c>
       <c r="E18" s="22" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>88</v>
@@ -10507,7 +10507,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>155</v>
@@ -10516,7 +10516,7 @@
         <v>8</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>88</v>
@@ -10530,7 +10530,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>155</v>
@@ -10539,7 +10539,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>88</v>
@@ -10553,7 +10553,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>155</v>
@@ -10562,7 +10562,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G21" s="22" t="s">
         <v>88</v>
@@ -10576,7 +10576,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>155</v>
@@ -10585,7 +10585,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G22" s="22" t="s">
         <v>88</v>
@@ -10599,7 +10599,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>155</v>
@@ -10608,7 +10608,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>88</v>
@@ -10622,7 +10622,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>155</v>
@@ -10631,7 +10631,7 @@
         <v>88</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G24" s="22" t="s">
         <v>88</v>
@@ -10645,7 +10645,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>155</v>
@@ -10654,7 +10654,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>88</v>
@@ -10677,7 +10677,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>88</v>
@@ -10691,7 +10691,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>30</v>
@@ -10700,7 +10700,7 @@
         <v>8</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>88</v>
@@ -10723,7 +10723,7 @@
         <v>8</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>88</v>
@@ -10746,7 +10746,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G29" s="22" t="s">
         <v>88</v>
@@ -10769,7 +10769,7 @@
         <v>8</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>88</v>
@@ -10792,7 +10792,7 @@
         <v>8</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G31" s="22" t="s">
         <v>88</v>
@@ -10806,7 +10806,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>17</v>
@@ -10815,7 +10815,7 @@
         <v>8</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G32" s="22" t="s">
         <v>88</v>
@@ -10838,7 +10838,7 @@
         <v>88</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G33" s="22" t="s">
         <v>88</v>
@@ -10861,7 +10861,7 @@
         <v>8</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G34" s="22" t="s">
         <v>88</v>
@@ -10875,7 +10875,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>14</v>
@@ -10884,7 +10884,7 @@
         <v>88</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G35" s="22" t="s">
         <v>88</v>
@@ -10898,7 +10898,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>14</v>
@@ -10907,7 +10907,7 @@
         <v>88</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G36" s="22" t="s">
         <v>88</v>
@@ -10921,7 +10921,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>14</v>
@@ -10930,7 +10930,7 @@
         <v>88</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G37" s="22" t="s">
         <v>88</v>
@@ -10953,7 +10953,7 @@
         <v>88</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G38" s="22" t="s">
         <v>88</v>
@@ -10974,7 +10974,7 @@
         <v>8</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>8</v>
@@ -11007,7 +11007,7 @@
       </c>
       <c r="B41" s="22"/>
       <c r="C41" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>6</v>
@@ -11016,7 +11016,7 @@
         <v>8</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G41" s="22" t="s">
         <v>8</v>
@@ -11028,7 +11028,7 @@
       </c>
       <c r="B42" s="22"/>
       <c r="C42" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>6</v>
@@ -11037,7 +11037,7 @@
         <v>8</v>
       </c>
       <c r="F42" s="26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G42" s="22" t="s">
         <v>8</v>
@@ -11130,7 +11130,7 @@
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>8</v>
@@ -11151,7 +11151,7 @@
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -11165,7 +11165,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>17</v>
@@ -11174,7 +11174,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -11188,7 +11188,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>158</v>
@@ -11197,7 +11197,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -11211,7 +11211,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>163</v>
@@ -11220,7 +11220,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -11234,7 +11234,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>41</v>
@@ -11243,7 +11243,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -11266,7 +11266,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -11280,7 +11280,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>6</v>
@@ -11289,7 +11289,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -11303,7 +11303,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>82</v>
@@ -11312,7 +11312,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -11326,7 +11326,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>14</v>
@@ -11335,7 +11335,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -11349,16 +11349,16 @@
         <v>13</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>294</v>
-      </c>
       <c r="E13" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -11372,7 +11372,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>155</v>
@@ -11381,7 +11381,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -11395,7 +11395,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>155</v>
@@ -11404,7 +11404,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -11418,16 +11418,16 @@
         <v>16</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -11441,7 +11441,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>30</v>
@@ -11450,7 +11450,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -11464,7 +11464,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>30</v>
@@ -11473,7 +11473,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>88</v>
@@ -11487,7 +11487,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>155</v>
@@ -11496,7 +11496,7 @@
         <v>8</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -11510,7 +11510,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>155</v>
@@ -11519,7 +11519,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -11533,7 +11533,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>155</v>
@@ -11542,7 +11542,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -11556,7 +11556,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>30</v>
@@ -11565,7 +11565,7 @@
         <v>8</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -11579,7 +11579,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>155</v>
@@ -11588,7 +11588,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -11602,7 +11602,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>155</v>
@@ -11611,7 +11611,7 @@
         <v>88</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>88</v>
@@ -11625,7 +11625,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>155</v>
@@ -11634,7 +11634,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>88</v>
@@ -11648,7 +11648,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>155</v>
@@ -11657,7 +11657,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>88</v>
@@ -11680,7 +11680,7 @@
         <v>88</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>88</v>
@@ -11703,13 +11703,13 @@
         <v>8</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="224.25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="207" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>28</v>
       </c>
@@ -11726,7 +11726,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>88</v>
@@ -11749,7 +11749,7 @@
         <v>8</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>88</v>
@@ -11772,7 +11772,7 @@
         <v>8</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>88</v>
@@ -11786,7 +11786,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>82</v>
@@ -11795,7 +11795,7 @@
         <v>88</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>88</v>
@@ -11809,7 +11809,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>17</v>
@@ -11818,7 +11818,7 @@
         <v>8</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>88</v>
@@ -11832,7 +11832,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>17</v>
@@ -11841,7 +11841,7 @@
         <v>88</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>88</v>
@@ -11855,7 +11855,7 @@
         <v>88</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>72</v>
@@ -11864,7 +11864,7 @@
         <v>8</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>88</v>
@@ -11887,7 +11887,7 @@
         <v>88</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>88</v>
@@ -11910,7 +11910,7 @@
         <v>8</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>88</v>
@@ -11924,7 +11924,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>78</v>
@@ -11933,7 +11933,7 @@
         <v>88</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>88</v>
@@ -11947,7 +11947,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>78</v>
@@ -11956,7 +11956,7 @@
         <v>88</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>88</v>
@@ -11970,7 +11970,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>14</v>
@@ -11979,7 +11979,7 @@
         <v>88</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>88</v>
@@ -11993,7 +11993,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>14</v>
@@ -12002,7 +12002,7 @@
         <v>88</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>88</v>
@@ -12016,7 +12016,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>14</v>
@@ -12025,7 +12025,7 @@
         <v>88</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>88</v>
@@ -12039,7 +12039,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>30</v>
@@ -12048,7 +12048,7 @@
         <v>88</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>88</v>
@@ -12062,7 +12062,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>41</v>
@@ -12071,7 +12071,7 @@
         <v>88</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G44" s="17" t="s">
         <v>88</v>
@@ -12085,7 +12085,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>17</v>
@@ -12094,7 +12094,7 @@
         <v>88</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>88</v>
@@ -12108,7 +12108,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>14</v>
@@ -12117,7 +12117,7 @@
         <v>88</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>88</v>
@@ -12140,7 +12140,7 @@
         <v>88</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>88</v>
@@ -12161,7 +12161,7 @@
         <v>8</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>8</v>
@@ -12232,14 +12232,14 @@
       </c>
       <c r="B52" s="17"/>
       <c r="C52" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>8</v>
@@ -12263,8 +12263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF4259E-5FE0-4614-AFBC-0BC3EDCF6526}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -12342,7 +12342,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>8</v>
@@ -12356,7 +12356,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>82</v>
@@ -12365,7 +12365,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>88</v>
@@ -12379,7 +12379,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>17</v>
@@ -12388,7 +12388,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -12402,7 +12402,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>82</v>
@@ -12411,7 +12411,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -12425,7 +12425,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>82</v>
@@ -12434,7 +12434,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -12448,7 +12448,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>44</v>
@@ -12457,7 +12457,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -12471,7 +12471,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>44</v>
@@ -12480,7 +12480,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -12494,7 +12494,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>78</v>
@@ -12503,7 +12503,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -12517,7 +12517,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>17</v>
@@ -12526,7 +12526,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -12549,7 +12549,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -12570,7 +12570,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>8</v>
@@ -12657,8 +12657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22712841-8BD7-4CFF-A03A-A40A4AAE3B2F}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -12727,7 +12727,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D3" s="35" t="s">
         <v>44</v>
@@ -12736,7 +12736,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>88</v>
@@ -12750,7 +12750,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D4" s="35" t="s">
         <v>44</v>
@@ -12759,7 +12759,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G4" s="34" t="s">
         <v>88</v>
@@ -12773,7 +12773,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D5" s="35" t="s">
         <v>44</v>
@@ -12782,7 +12782,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>88</v>
@@ -12796,7 +12796,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>44</v>
@@ -12805,7 +12805,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>88</v>
@@ -12819,7 +12819,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D7" s="35" t="s">
         <v>78</v>
@@ -12828,7 +12828,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G7" s="34" t="s">
         <v>88</v>
@@ -12842,7 +12842,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>17</v>
@@ -12851,7 +12851,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G8" s="34" t="s">
         <v>88</v>
@@ -12874,7 +12874,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G9" s="34" t="s">
         <v>88</v>
@@ -12895,7 +12895,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G10" s="34" t="s">
         <v>8</v>
@@ -13010,7 +13010,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>8</v>
@@ -13047,7 +13047,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>210</v>
@@ -13056,7 +13056,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>88</v>
@@ -13070,7 +13070,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>210</v>
@@ -13079,7 +13079,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>88</v>
@@ -13093,7 +13093,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>27</v>
@@ -13102,7 +13102,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>88</v>
@@ -13116,7 +13116,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>14</v>
@@ -13125,7 +13125,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>88</v>
@@ -13139,7 +13139,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>14</v>
@@ -13148,7 +13148,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>88</v>
@@ -13162,7 +13162,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>14</v>
@@ -13171,7 +13171,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>88</v>
@@ -13185,7 +13185,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>158</v>
@@ -13194,7 +13194,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>88</v>
@@ -13208,7 +13208,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>210</v>
@@ -13217,7 +13217,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>88</v>
@@ -13231,7 +13231,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>210</v>
@@ -13240,7 +13240,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>88</v>
@@ -13254,7 +13254,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>14</v>
@@ -13263,7 +13263,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>88</v>
@@ -13277,7 +13277,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>210</v>
@@ -13286,7 +13286,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>88</v>
@@ -13300,7 +13300,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>14</v>
@@ -13309,7 +13309,7 @@
         <v>88</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>88</v>
@@ -13323,7 +13323,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>210</v>
@@ -13332,7 +13332,7 @@
         <v>88</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>88</v>
@@ -13346,7 +13346,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>14</v>
@@ -13355,7 +13355,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>88</v>
@@ -13369,16 +13369,16 @@
         <v>18</v>
       </c>
       <c r="C19" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>455</v>
-      </c>
       <c r="E19" s="17" t="s">
         <v>88</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>88</v>
@@ -13392,7 +13392,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>14</v>
@@ -13401,7 +13401,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>88</v>
@@ -13415,7 +13415,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>210</v>
@@ -13424,7 +13424,7 @@
         <v>88</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>88</v>
@@ -13438,7 +13438,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>210</v>
@@ -13447,7 +13447,7 @@
         <v>88</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>88</v>
@@ -13461,7 +13461,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>14</v>
@@ -13470,7 +13470,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>88</v>
@@ -13484,7 +13484,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>210</v>
@@ -13493,7 +13493,7 @@
         <v>88</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>88</v>
@@ -13507,7 +13507,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>210</v>
@@ -13516,7 +13516,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>88</v>
@@ -13530,7 +13530,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>14</v>
@@ -13539,7 +13539,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>88</v>
@@ -13553,7 +13553,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>210</v>
@@ -13562,7 +13562,7 @@
         <v>88</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>88</v>
@@ -13576,7 +13576,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>210</v>
@@ -13585,7 +13585,7 @@
         <v>88</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>88</v>
@@ -13599,7 +13599,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>27</v>
@@ -13608,7 +13608,7 @@
         <v>88</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>88</v>
@@ -13622,7 +13622,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>14</v>
@@ -13631,7 +13631,7 @@
         <v>88</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>88</v>
@@ -13645,7 +13645,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>30</v>
@@ -13654,7 +13654,7 @@
         <v>88</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>88</v>
@@ -13677,7 +13677,7 @@
         <v>88</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>88</v>
@@ -13698,7 +13698,7 @@
         <v>8</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>8</v>

</xml_diff>